<commit_message>
improved compressed Liquid interpolation
</commit_message>
<xml_diff>
--- a/src/main/resources/CompressedLiquid.xlsx
+++ b/src/main/resources/CompressedLiquid.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammed Azab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CS Projects\Thermodynamics_Java_Library\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646B20D2-31E8-45BF-A71D-F1D2C897E9A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8990221F-B0E2-4497-80F0-CBE21DFEA6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="7">
   <si>
     <t>P</t>
   </si>
@@ -409,8 +409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="I106" sqref="I106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2692,17 +2692,17 @@
       <c r="B114" s="1">
         <v>380</v>
       </c>
-      <c r="C114" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>6</v>
+      <c r="C114" s="1">
+        <v>1.5884E-3</v>
+      </c>
+      <c r="D114" s="1">
+        <v>1667.1</v>
+      </c>
+      <c r="E114" s="1">
+        <v>1746.5</v>
+      </c>
+      <c r="F114" s="1">
+        <v>3.8102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>